<commit_message>
adding industry composition in last year bar chart
Yet to resolve the momentary no aggregate rows warning message
</commit_message>
<xml_diff>
--- a/dashboard_development_tracker.xlsx
+++ b/dashboard_development_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FFC228-1CD0-4E78-8BA8-465D0E78FE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3048E576-9EA1-42D1-A6C1-4EF25C05C3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="4890" windowWidth="17280" windowHeight="9105" xr2:uid="{9C48A006-AFAD-4054-8C64-BDCDCF328DCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C48A006-AFAD-4054-8C64-BDCDCF328DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Aesthetics/ Functionality</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Run with Action Button</t>
+  </si>
+  <si>
+    <t>Just need to push this update across the other tabs, when time permits</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -384,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -471,11 +477,162 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -796,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62358F1-E889-4A47-AEF3-E1CB36E9A86E}">
-  <dimension ref="B2:G31"/>
+  <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -807,13 +964,15 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="98.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="18" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="38" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
@@ -824,309 +983,399 @@
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="32">
+        <v>1</v>
+      </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33">
+        <v>2</v>
+      </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="33">
+        <v>1</v>
+      </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33">
+        <v>3</v>
+      </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33">
+        <v>2</v>
+      </c>
       <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="C8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33">
+        <v>2</v>
+      </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="33">
+        <v>1</v>
+      </c>
       <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33">
+        <v>2</v>
+      </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="D11" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="33">
+        <v>1</v>
+      </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G11" s="14"/>
+      <c r="H11" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G12" s="29"/>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="16"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36">
+        <v>1</v>
+      </c>
       <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
       <c r="C15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33">
+        <v>1</v>
+      </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="12"/>
       <c r="C16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33">
+        <v>1</v>
+      </c>
       <c r="F16" s="14"/>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="12"/>
       <c r="C17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33">
+        <v>1</v>
+      </c>
       <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
       <c r="C18" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33">
+        <v>1</v>
+      </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="12"/>
       <c r="C19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="2:7" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="2:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
       <c r="C20" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33">
+        <v>3</v>
+      </c>
       <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="14"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
       <c r="C21" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33">
+        <v>3</v>
+      </c>
       <c r="F21" s="14"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
       <c r="C22" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33">
+        <v>3</v>
+      </c>
       <c r="F22" s="14"/>
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
       <c r="C23" s="31"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
       <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="29"/>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="16"/>
       <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36">
+        <v>2</v>
+      </c>
       <c r="F25" s="22"/>
-      <c r="G25" s="23" t="s">
+      <c r="G25" s="22"/>
+      <c r="H25" s="23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
       <c r="C26" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33">
+        <v>2</v>
+      </c>
       <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
       <c r="C27" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33">
+        <v>2</v>
+      </c>
       <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="14"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="C28" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33">
+        <v>2</v>
+      </c>
       <c r="F28" s="14"/>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
       <c r="C29" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33">
+        <v>2</v>
+      </c>
       <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="14"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
       <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="14"/>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="16"/>
       <c r="C31" s="24"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="26"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D30">
+  <conditionalFormatting sqref="E3:E31">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D31">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",D3)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Tidying Nested Pie & Final Year charts
</commit_message>
<xml_diff>
--- a/dashboard_development_tracker.xlsx
+++ b/dashboard_development_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3048E576-9EA1-42D1-A6C1-4EF25C05C3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E916B16-5BED-401B-94C7-1D7BA05EDE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C48A006-AFAD-4054-8C64-BDCDCF328DCF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Aesthetics/ Functionality</t>
   </si>
@@ -502,137 +502,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -956,7 +826,7 @@
   <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1149,7 +1019,9 @@
       <c r="C14" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="32" t="s">
+        <v>31</v>
+      </c>
       <c r="E14" s="36">
         <v>1</v>
       </c>
@@ -1175,7 +1047,9 @@
       <c r="C16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="33" t="s">
+        <v>31</v>
+      </c>
       <c r="E16" s="33">
         <v>1</v>
       </c>

</xml_diff>